<commit_message>
slight change to analysis
</commit_message>
<xml_diff>
--- a/data_analysis/DataAnalysisCrudeRefined (Cumulative Calculations).xlsx
+++ b/data_analysis/DataAnalysisCrudeRefined (Cumulative Calculations).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Dropbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="24" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="32" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Crude Fruits and Veg" sheetId="6" r:id="rId1"/>
@@ -40,10 +40,18 @@
     <sheet name="Refined Fats and Oils" sheetId="32" r:id="rId26"/>
     <sheet name="Refined Fish and Seafood" sheetId="33" r:id="rId27"/>
     <sheet name="Refined Fresh Fruit" sheetId="34" r:id="rId28"/>
-    <sheet name="Main" sheetId="1" r:id="rId29"/>
+    <sheet name="Refined Fresh Fruit and Veg" sheetId="35" r:id="rId29"/>
+    <sheet name="Refined Fresh Veg" sheetId="36" r:id="rId30"/>
+    <sheet name="Refined Meats Poultry" sheetId="37" r:id="rId31"/>
+    <sheet name="Refined Nonalcohlic" sheetId="38" r:id="rId32"/>
+    <sheet name="Refined Other Meats" sheetId="39" r:id="rId33"/>
+    <sheet name="Refined Pork" sheetId="40" r:id="rId34"/>
+    <sheet name="Refined Poultry" sheetId="41" r:id="rId35"/>
+    <sheet name="Refined Sugar and Sweets" sheetId="42" r:id="rId36"/>
+    <sheet name="Main" sheetId="1" r:id="rId37"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">Main!$J$25:$AA$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="36" hidden="1">Main!$J$25:$AA$26</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="66">
   <si>
     <t>Year</t>
   </si>
@@ -5354,10 +5362,2044 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.24435604495380292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.9709876705464952E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.6128086587802985E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.6928831370491397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>24.247862477413548</v>
+      </c>
+      <c r="D12" s="1">
+        <v>24.247862477413548</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.7780432935902726</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.19313698400499996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>381.84680418925302</v>
+      </c>
+      <c r="D13" s="1">
+        <v>13.637385863901894</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>406.09466666666657</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.5472450770412625</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.70313600856736047</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.0448917902366768</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2.4529943686517366E-5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2.106936255438479</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4.9875538986440464</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2.106936255438479</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4.9875538986440464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4.0713539128661831E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.0532874348859554E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.3334328980455958</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.19313698400500029</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2.1830218747078904E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.10325729700440256</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.1830218747078904E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.10325729700440256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.49281555829856949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.24286717450113074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.21582671644759971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.1356660011707147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>88.310912133845306</v>
+      </c>
+      <c r="D12" s="1">
+        <v>88.310912133845306</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8.9816220575973649</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5.6601418452295674E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>275.30723558514234</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9.8324012708979414</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>363.61814771898764</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.0969681994487548</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.59347450252290002</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.5333753860265302</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.4452504106917195E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.88129079000746646</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.3126456088900431</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.88129079000746646</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.3126456088900431</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>7.2214892276589379E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2.4096245520653141E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.9969354443493383</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5.6601418452295682E-3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.2855970861631818E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.12157381369154693</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.2855970861631818E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.12157381369154693</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.15439637626565372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.3838241003965324E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-1.1024678960178771E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.3979697126441444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>13.225585750017444</v>
+      </c>
+      <c r="D12" s="1">
+        <v>13.225585750017444</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.68377063735575039</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.41528291907026238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>541.57985261338615</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19.34213759333522</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>554.8054383634036</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.6057444952893039</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.83738660412085397</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.3059495787789226</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.8410874993701225E-4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.8904357949644794</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5.3210531956141285</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.8904357949644794</v>
+      </c>
+      <c r="I17" s="1">
+        <v>5.3210531956141285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3.0068349102352936E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.636255241305969E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.82690424920649475</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.41528291907026027</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-4.441696295446243E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.10455366115916831</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-4.441696295446243E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.10455366115916831</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.50634382658352917</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.25638407071925107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.22982635895922435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.3257601960933063</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>52.219204653715423</v>
+      </c>
+      <c r="D12" s="1">
+        <v>52.219204653715423</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9.6538464245683517</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.3029440709852458E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>151.4564937124953</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.4091604897319749</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>203.67569836621072</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.5741803637520588</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.44283170641371111</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.8129992194984261</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.0304132436083553E-6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.667080733720838</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.4812799937832795</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.667080733720838</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.4812799937832795</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5.9747158068402174E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.9229458717623903E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.1070639556610913</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4.3029440709852458E-3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.035739749836455E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>9.9136918638439792E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.035739749836455E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>9.9136918638439792E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.12393885679373579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5360840223338147E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-1.9804844054399775E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.383649868772173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.4818802598811942</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.4818802598811942</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.43681334627298923</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.5140662471228199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>159.09002751313275</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.6817866968975981</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>161.57190777301395</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.3311827824567506</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.45385407345704382</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.9330634234854869</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.6245193736031082E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.40150485705447847</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2.2608607078590226</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.40150485705447847</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.2608607078590226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.3025444071574755E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.970809235871248E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.66091856251203918</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.51406624712282434</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2.734475306717217E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5.3395641210321684E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.734475306717217E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5.3395641210321684E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.33572631547158943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.11271215890012917</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.1023307432276634E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.0686082831160286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>15.220215031573389</v>
+      </c>
+      <c r="D12" s="1">
+        <v>15.220215031573389</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.5568395091400693</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6.9713677341553246E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>119.81592641133483</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4.2791402289762441</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>135.03614144290822</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.4493294237586252</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.39386921207635017</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.2186364119362318</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.0182722726323877E-6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.6425249168081637</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.2561339307090869</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.6425249168081637</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.2561339307090869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3.2256149267112941E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.7103318583718111E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.8859585120410438</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6.9713677341553218E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2.7784106681745663E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6.7290709202400448E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.7784106681745663E-3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>6.7290709202400448E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.56744086203575383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.32198913190787942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.29777445804744657</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.9712295882163215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>209.70683242164625</v>
+      </c>
+      <c r="D12" s="1">
+        <v>209.70683242164625</v>
+      </c>
+      <c r="E12" s="1">
+        <v>13.297273123055117</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.0746501700430544E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>441.57860438509374</v>
+      </c>
+      <c r="D13" s="1">
+        <v>15.770664442324776</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>651.28543680673999</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.5859769790463458</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.75613400644848805</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.0974813532003087</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4.5102668051769684E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.7106680083011323E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.1348472780096803</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3.7106680083011323E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.1348472780096803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.11973149802791089</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.2834251593558822E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.6465426259753371</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.0746501700430575E-3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5.2473582568163105E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.18698941348765868</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5.2473582568163105E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.18698941348765868</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.10949088170982738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.198825317759541E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-2.3297880637490467E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.025503060830355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.1099042844077758</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.1099042844077758</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.33974402637644796</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.56464225336435403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>256.30272559062769</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9.1536687710938462</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>259.41262987503546</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.3224918037991369</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.57606484341675512</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.0316499615285952</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.8599643220904595E-4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.1424764644070964</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.5025071431911776</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.1424764644070964</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.5025071431911776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.4580608110294834E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2.5014954811767711E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.58287565258505769</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.56464225336434892</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-3.6660203977815456E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6.5821420198405131E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-3.6660203977815456E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>6.5821420198405131E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.4165851802008489E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.8398839331663698E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-3.5109440592636341E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.8065937119565423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.3399468279906159E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.3399468279906159E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.6361229781158417E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.89913365919213561</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>91.385863522265709</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.2637808400809183</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>91.439262990545615</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.2854675987335558</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.34398085305863607</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.6441709717603601</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.2938329987127181E-7</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.5808547626874252</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2.9900804347796863</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.5808547626874252</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.9900804347796863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.9106036028152453E-3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.4936973838464273E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.12791102290714607</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.89913365919215393</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2.8686400284703699E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.2507607490334191E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.8686400284703699E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>3.2507607490334191E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8571,6 +10613,30 @@
       <c r="S43">
         <v>0.21795744674323886</v>
       </c>
+      <c r="T43">
+        <v>0.19313698400499996</v>
+      </c>
+      <c r="U43">
+        <v>0.41528291907026238</v>
+      </c>
+      <c r="V43">
+        <v>4.3029440709852458E-3</v>
+      </c>
+      <c r="W43">
+        <v>0.5140662471228199</v>
+      </c>
+      <c r="X43">
+        <v>6.9713677341553246E-2</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>1.0746501700430544E-3</v>
+      </c>
+      <c r="Z43">
+        <v>0.56464225336435403</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>0.89913365919213561</v>
+      </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -8633,232 +10699,6 @@
       <c r="B50">
         <f>AVERAGE(J33:AA33)</f>
         <v>2.9541192628937472</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.49281555829856949</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.24286717450113074</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.21582671644759971</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.1356660011707147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>88.310912133845306</v>
-      </c>
-      <c r="D12" s="1">
-        <v>88.310912133845306</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8.9816220575973649</v>
-      </c>
-      <c r="F12" s="1">
-        <v>5.6601418452295674E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="1">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1">
-        <v>275.30723558514234</v>
-      </c>
-      <c r="D13" s="1">
-        <v>9.8324012708979414</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2">
-        <v>363.61814771898764</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2.0969681994487548</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.59347450252290002</v>
-      </c>
-      <c r="D17" s="1">
-        <v>3.5333753860265302</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1.4452504106917195E-3</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.88129079000746646</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3.3126456088900431</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0.88129079000746646</v>
-      </c>
-      <c r="I17" s="1">
-        <v>3.3126456088900431</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2">
-        <v>7.2214892276589379E-2</v>
-      </c>
-      <c r="C18" s="2">
-        <v>2.4096245520653141E-2</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2.9969354443493383</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5.6601418452295682E-3</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2.2855970861631818E-2</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.12157381369154693</v>
-      </c>
-      <c r="H18" s="2">
-        <v>2.2855970861631818E-2</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.12157381369154693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>